<commit_message>
Add Hamptons and Hampton Court blaze.
</commit_message>
<xml_diff>
--- a/Fires.xlsx
+++ b/Fires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drrja\OneDrive\Documents\GitHub\CroydonRockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B47BB0B-153E-4A1B-8B88-E06C58E7B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB814B-5E87-40CB-BE90-CE42405EF39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="330" windowWidth="21840" windowHeight="15015" xr2:uid="{48518D89-2145-4A98-8BBC-807CBE7E41BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48518D89-2145-4A98-8BBC-807CBE7E41BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>BBC NEWS | England | London | Blaze ravages historic Cutty Sark</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>BBC NEWS | England | London | Cutty Sark blaze was accidental</t>
+  </si>
+  <si>
+    <t>Explosions heard as 100 firefighters tackle huge blaze at historic boat yards on Thames island near Hampton Court (thesun.co.uk)</t>
+  </si>
+  <si>
+    <t>https://twitter.com/LondonFire/status/1389282224588132353?s=20</t>
+  </si>
+  <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>Worcester Park fire: What happened and were there any deaths? (thesun.co.uk)</t>
   </si>
 </sst>
 </file>
@@ -50,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,11 +102,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,43 +423,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB2BD42-0128-4359-B0E9-35BD0D02113E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>39223</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="C2" s="4">
         <v>0.15625</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>43717</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3-1/24</f>
+        <v>2.3611111111111117E-2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44319</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://news.bbc.co.uk/1/hi/england/london/6675381.stm" xr:uid="{956E4310-A995-4091-8BC2-8EC234D3141F}"/>
-    <hyperlink ref="D2" r:id="rId2" display="http://news.bbc.co.uk/1/hi/england/london/7643420.stm" xr:uid="{C4DBF97F-1142-4D61-ACC1-7967395D2BE1}"/>
+    <hyperlink ref="E2" r:id="rId1" display="http://news.bbc.co.uk/1/hi/england/london/6675381.stm" xr:uid="{956E4310-A995-4091-8BC2-8EC234D3141F}"/>
+    <hyperlink ref="F2" r:id="rId2" display="http://news.bbc.co.uk/1/hi/england/london/7643420.stm" xr:uid="{C4DBF97F-1142-4D61-ACC1-7967395D2BE1}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://www.thesun.co.uk/news/14840746/firefighters-tackle-huge-blaze-at-historic-boat-house/" xr:uid="{F7242755-60E7-45D1-A927-7B38B5BDCF70}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{BCDC70FD-4738-411B-BBCF-7BF0A1D01C77}"/>
+    <hyperlink ref="E3" r:id="rId5" display="https://www.thesun.co.uk/news/9892888/worcester-park-fire-cause-sherbrooke-hamptons-london/" xr:uid="{E6302F5A-B597-4D74-A8D0-28D19D763FE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Hampton Court Fire
</commit_message>
<xml_diff>
--- a/Fires.xlsx
+++ b/Fires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drrja\OneDrive\Documents\GitHub\CroydonRockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB814B-5E87-40CB-BE90-CE42405EF39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BC2A29-F7CC-4B3A-BE3E-59CE383C09CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48518D89-2145-4A98-8BBC-807CBE7E41BF}"/>
+    <workbookView xWindow="29520" yWindow="300" windowWidth="21840" windowHeight="15015" xr2:uid="{48518D89-2145-4A98-8BBC-807CBE7E41BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>BBC NEWS | England | London | Blaze ravages historic Cutty Sark</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Worcester Park fire: What happened and were there any deaths? (thesun.co.uk)</t>
+  </si>
+  <si>
+    <t>The Hampton Court fire. March 1986. – A retired London Fireman (home.blog)</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB2BD42-0128-4359-B0E9-35BD0D02113E}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,59 +450,68 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>39223</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.19791666666666666</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.15625</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>31502</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43717</v>
+        <v>39223</v>
       </c>
       <c r="B3" s="4">
-        <v>6.5277777777777782E-2</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="C3" s="4">
-        <f>B3-1/24</f>
-        <v>2.3611111111111117E-2</v>
-      </c>
+        <v>0.15625</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
+        <v>43717</v>
+      </c>
+      <c r="B4" s="4">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <f>B4-1/24</f>
+        <v>2.3611111111111117E-2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>44319</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="http://news.bbc.co.uk/1/hi/england/london/6675381.stm" xr:uid="{956E4310-A995-4091-8BC2-8EC234D3141F}"/>
-    <hyperlink ref="F2" r:id="rId2" display="http://news.bbc.co.uk/1/hi/england/london/7643420.stm" xr:uid="{C4DBF97F-1142-4D61-ACC1-7967395D2BE1}"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://www.thesun.co.uk/news/14840746/firefighters-tackle-huge-blaze-at-historic-boat-house/" xr:uid="{F7242755-60E7-45D1-A927-7B38B5BDCF70}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{BCDC70FD-4738-411B-BBCF-7BF0A1D01C77}"/>
-    <hyperlink ref="E3" r:id="rId5" display="https://www.thesun.co.uk/news/9892888/worcester-park-fire-cause-sherbrooke-hamptons-london/" xr:uid="{E6302F5A-B597-4D74-A8D0-28D19D763FE0}"/>
+    <hyperlink ref="E3" r:id="rId1" display="http://news.bbc.co.uk/1/hi/england/london/6675381.stm" xr:uid="{956E4310-A995-4091-8BC2-8EC234D3141F}"/>
+    <hyperlink ref="F3" r:id="rId2" display="http://news.bbc.co.uk/1/hi/england/london/7643420.stm" xr:uid="{C4DBF97F-1142-4D61-ACC1-7967395D2BE1}"/>
+    <hyperlink ref="E5" r:id="rId3" display="https://www.thesun.co.uk/news/14840746/firefighters-tackle-huge-blaze-at-historic-boat-house/" xr:uid="{F7242755-60E7-45D1-A927-7B38B5BDCF70}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{BCDC70FD-4738-411B-BBCF-7BF0A1D01C77}"/>
+    <hyperlink ref="E4" r:id="rId5" display="https://www.thesun.co.uk/news/9892888/worcester-park-fire-cause-sherbrooke-hamptons-london/" xr:uid="{E6302F5A-B597-4D74-A8D0-28D19D763FE0}"/>
+    <hyperlink ref="E2" r:id="rId6" display="https://beyondtheflamesandmore.home.blog/2021/03/31/the-hampton-court-fire-march-1986/" xr:uid="{CD7D0B1F-C039-4D49-9DF9-40FF0EA0D61D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>